<commit_message>
Change to reading .xlsx file directly with pandas, add code for constructing Y matrix, alter directory structure for easier file access
</commit_message>
<xml_diff>
--- a/data/system_basecase.xlsx
+++ b/data/system_basecase.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Documents/Work/UW/Teaching/EE454/2021/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F831088-659A-1344-8D80-D7ABFD8C0C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1A68B2-B6F7-EB4A-AF68-ED7D8F86DC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>Bus #</t>
   </si>
@@ -74,15 +74,25 @@
   </si>
   <si>
     <t>To</t>
+  </si>
+  <si>
+    <t>Btotal, p.u.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -97,7 +107,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -105,12 +115,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -667,20 +714,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="4" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -694,10 +741,13 @@
         <v>10</v>
       </c>
       <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -710,11 +760,14 @@
       <c r="D2">
         <v>5.917E-2</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
+        <v>5.28E-2</v>
+      </c>
+      <c r="F2">
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -727,28 +780,34 @@
       <c r="D3">
         <v>0.22303999999999999</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
+        <v>4.9200000000000001E-2</v>
+      </c>
+      <c r="F3">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>4.6989999999999997E-2</v>
       </c>
       <c r="D4">
         <v>0.19797000000000001</v>
       </c>
-      <c r="E4">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4" s="3">
+        <v>4.3799999999999999E-2</v>
+      </c>
+      <c r="F4">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -761,11 +820,14 @@
       <c r="D5">
         <v>0.17632</v>
       </c>
-      <c r="E5">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5" s="3">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="F5">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -778,11 +840,14 @@
       <c r="D6">
         <v>0.17388000000000001</v>
       </c>
-      <c r="E6">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E6" s="3">
+        <v>3.4599999999999999E-2</v>
+      </c>
+      <c r="F6">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -795,11 +860,14 @@
       <c r="D7">
         <v>0.17102999999999999</v>
       </c>
-      <c r="E7">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E7" s="3">
+        <v>1.2800000000000001E-2</v>
+      </c>
+      <c r="F7">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -812,11 +880,14 @@
       <c r="D8">
         <v>4.2110000000000002E-2</v>
       </c>
-      <c r="E8">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -829,11 +900,14 @@
       <c r="D9">
         <v>0.55618000000000001</v>
       </c>
-      <c r="E9">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
@@ -846,11 +920,14 @@
       <c r="D10">
         <v>0.25202000000000002</v>
       </c>
-      <c r="E10">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
@@ -863,11 +940,14 @@
       <c r="D11">
         <v>0.19889999999999999</v>
       </c>
-      <c r="E11">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -880,11 +960,14 @@
       <c r="D12">
         <v>0.25580999999999998</v>
       </c>
-      <c r="E12">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
@@ -897,11 +980,14 @@
       <c r="D13">
         <v>0.13027</v>
       </c>
-      <c r="E13">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7</v>
       </c>
@@ -914,11 +1000,14 @@
       <c r="D14">
         <v>8.4500000000000006E-2</v>
       </c>
-      <c r="E14">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7</v>
       </c>
@@ -931,11 +1020,14 @@
       <c r="D15">
         <v>0.27038000000000001</v>
       </c>
-      <c r="E15">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>8</v>
       </c>
@@ -948,11 +1040,14 @@
       <c r="D16">
         <v>0.19206999999999999</v>
       </c>
-      <c r="E16">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10</v>
       </c>
@@ -965,11 +1060,14 @@
       <c r="D17">
         <v>0.19988</v>
       </c>
-      <c r="E17">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>11</v>
       </c>
@@ -982,7 +1080,10 @@
       <c r="D18">
         <v>0.34802</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18">
         <v>9999</v>
       </c>
     </row>

</xml_diff>